<commit_message>
substitui arquivo RGPS de 2019, em razão de nova UO para o RGPS :unamused:
</commit_message>
<xml_diff>
--- a/dados/tg_ Base Siafi 2019 so RGPS Pgtos Totais Esf-Acao-Mod.xlsx
+++ b/dados/tg_ Base Siafi 2019 so RGPS Pgtos Totais Esf-Acao-Mod.xlsx
@@ -19,7 +19,7 @@
     <t>Filtro do relatório:</t>
   </si>
   <si>
-    <t>({Item Informação} = 56:PAGAMENTOS TOTAIS (EXERCICIO E RAP)) E ({Órgão UGE - Orçam. Fiscal S/N} = PERTENCE) E ({Unidade Orçamentária} = 40904:FUNDO DO REGIME GERAL DA PREVID.SOCIAL- FRGPS, 55902:FUNDO DO REGIME GERAL DA PREVID.SOCIAL-FRGPS, 33904:FUNDO DO REGIME GERAL DA PREVIDENCIA SOCIAL) E ({Ano Lançamento} ({Número Ano}) = 2019)</t>
+    <t>({Item Informação} = 56:PAGAMENTOS TOTAIS (EXERCICIO E RAP)) E ({Órgão UGE - Orçam. Fiscal S/N} = PERTENCE) E ({Unidade Orçamentária} = 40904:FUNDO DO REGIME GERAL DA PREVID.SOCIAL- FRGPS, 55902:FUNDO DO REGIME GERAL DA PREVID.SOCIAL-FRGPS, 33904:FUNDO DO REGIME GERAL DA PREVIDENCIA SOCIAL, 25917:FUNDO DO REGIME GERAL DE PREVIDENCIA SOCIAL) E ({Ano Lançamento} ({Número Ano}) = 2019)</t>
   </si>
   <si>
     <t>Páginas:</t>
@@ -531,7 +531,7 @@
         <v>27</v>
       </c>
       <c r="U12" s="1">
-        <v>1133396.51</v>
+        <v>2194900.8</v>
       </c>
     </row>
     <row r="13">
@@ -596,7 +596,7 @@
         <v>37</v>
       </c>
       <c r="U13" s="1">
-        <v>1372340.26</v>
+        <v>6161800449.26</v>
       </c>
     </row>
     <row r="14">
@@ -661,7 +661,7 @@
         <v>49</v>
       </c>
       <c r="U14" s="1">
-        <v>467590.64</v>
+        <v>57482832.8299999</v>
       </c>
     </row>
     <row r="15">
@@ -726,7 +726,7 @@
         <v>51</v>
       </c>
       <c r="U15" s="1">
-        <v>997310.21</v>
+        <v>58038967.9499998</v>
       </c>
     </row>
     <row r="16">
@@ -791,7 +791,7 @@
         <v>53</v>
       </c>
       <c r="U16" s="1">
-        <v>772167.21</v>
+        <v>9251715.32999992</v>
       </c>
     </row>
     <row r="17">
@@ -921,7 +921,7 @@
         <v>27</v>
       </c>
       <c r="U18" s="1">
-        <v>503810873.04</v>
+        <v>572934223.48</v>
       </c>
     </row>
     <row r="19">
@@ -986,7 +986,7 @@
         <v>37</v>
       </c>
       <c r="U19" s="1">
-        <v>-946915260.39</v>
+        <v>956666330.04</v>
       </c>
     </row>
     <row r="20">
@@ -1051,7 +1051,7 @@
         <v>49</v>
       </c>
       <c r="U20" s="1">
-        <v>5951.18000000715</v>
+        <v>876046353.92</v>
       </c>
     </row>
     <row r="21">
@@ -1116,7 +1116,7 @@
         <v>51</v>
       </c>
       <c r="U21" s="1">
-        <v>59385.6699999869</v>
+        <v>940334079.67</v>
       </c>
     </row>
     <row r="22">
@@ -1181,7 +1181,7 @@
         <v>53</v>
       </c>
       <c r="U22" s="1">
-        <v>0</v>
+        <v>25452262.8099999</v>
       </c>
     </row>
     <row r="23">
@@ -1376,7 +1376,7 @@
         <v>37</v>
       </c>
       <c r="U25" s="1">
-        <v>0</v>
+        <v>483053256.24</v>
       </c>
     </row>
     <row r="26">
@@ -1441,7 +1441,7 @@
         <v>49</v>
       </c>
       <c r="U26" s="1">
-        <v>0</v>
+        <v>255969667.98</v>
       </c>
     </row>
     <row r="27">
@@ -1506,7 +1506,7 @@
         <v>51</v>
       </c>
       <c r="U27" s="1">
-        <v>0</v>
+        <v>242092703.06</v>
       </c>
     </row>
     <row r="28">
@@ -1571,7 +1571,7 @@
         <v>53</v>
       </c>
       <c r="U28" s="1">
-        <v>0</v>
+        <v>283156554.82</v>
       </c>
     </row>
     <row r="29">
@@ -1701,7 +1701,7 @@
         <v>27</v>
       </c>
       <c r="U30" s="1">
-        <v>-7395912500.65</v>
+        <v>45604902847.01</v>
       </c>
     </row>
     <row r="31">
@@ -1766,7 +1766,7 @@
         <v>37</v>
       </c>
       <c r="U31" s="1">
-        <v>-102324.150001526</v>
+        <v>27345470660.24</v>
       </c>
     </row>
     <row r="32">
@@ -1831,7 +1831,7 @@
         <v>49</v>
       </c>
       <c r="U32" s="1">
-        <v>237</v>
+        <v>36735225735.85</v>
       </c>
     </row>
     <row r="33">
@@ -1896,7 +1896,7 @@
         <v>51</v>
       </c>
       <c r="U33" s="1">
-        <v>0</v>
+        <v>36776283820.94</v>
       </c>
     </row>
     <row r="34">
@@ -1961,7 +1961,7 @@
         <v>53</v>
       </c>
       <c r="U34" s="1">
-        <v>302.399997711182</v>
+        <v>31619201138.78</v>
       </c>
     </row>
     <row r="35">
@@ -2091,7 +2091,7 @@
         <v>27</v>
       </c>
       <c r="U36" s="1">
-        <v>-4841779723.32</v>
+        <v>567052855.599998</v>
       </c>
     </row>
     <row r="37">
@@ -2156,7 +2156,7 @@
         <v>37</v>
       </c>
       <c r="U37" s="1">
-        <v>-13585.5000009537</v>
+        <v>18841702314.3</v>
       </c>
     </row>
     <row r="38">
@@ -2221,7 +2221,7 @@
         <v>49</v>
       </c>
       <c r="U38" s="1">
-        <v>0</v>
+        <v>9735751180.34</v>
       </c>
     </row>
     <row r="39">
@@ -2286,7 +2286,7 @@
         <v>51</v>
       </c>
       <c r="U39" s="1">
-        <v>0</v>
+        <v>9587040690.81</v>
       </c>
     </row>
     <row r="40">
@@ -2351,7 +2351,7 @@
         <v>53</v>
       </c>
       <c r="U40" s="1">
-        <v>0</v>
+        <v>5008188970.76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>